<commit_message>
Updating MIATE to version 3. Added CEDAR and GEO templates and new fields to the checklist
</commit_message>
<xml_diff>
--- a/checklist/MIATE-Checklist.xlsx
+++ b/checklist/MIATE-Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/MIATE/checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{E3226569-7E5F-48E9-B996-B5F931ABBD7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CFCD3235-78FB-4ABD-898B-901059CCFAFE}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{E3226569-7E5F-48E9-B996-B5F931ABBD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40E70923-061C-4375-92D9-59576ACFF38D}"/>
   <bookViews>
-    <workbookView xWindow="-54120" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60165" yWindow="2325" windowWidth="18405" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIATE-Checklist" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="129">
   <si>
     <t>ISA Section</t>
   </si>
@@ -382,16 +382,31 @@
     <t>Termination Conditions</t>
   </si>
   <si>
-    <t>Fasting duration</t>
-  </si>
-  <si>
     <t>Euthanasia method</t>
   </si>
   <si>
-    <t>Amount of time animals were fasted prior to euthanisation.</t>
-  </si>
-  <si>
     <t>Method used for euthanasia.</t>
+  </si>
+  <si>
+    <t>Administration volume</t>
+  </si>
+  <si>
+    <t>Organism supplier</t>
+  </si>
+  <si>
+    <t>Provide the name of the vendor for the organism</t>
+  </si>
+  <si>
+    <t>The volume in which the substance was administered</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>ad lib feeding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes or No </t>
   </si>
 </sst>
 </file>
@@ -1423,24 +1438,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="87" workbookViewId="0">
+      <selection activeCell="D62" sqref="D61:G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1472,7 +1487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>9</v>
       </c>
@@ -1486,7 +1501,7 @@
       <c r="I2" s="10"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
@@ -1500,7 +1515,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="19" t="s">
         <v>11</v>
@@ -1522,7 +1537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="19" t="s">
         <v>14</v>
@@ -1544,7 +1559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="19" t="s">
         <v>10</v>
@@ -1566,7 +1581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="19" t="s">
         <v>16</v>
@@ -1588,7 +1603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="19" t="s">
         <v>17</v>
@@ -1610,7 +1625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>18</v>
       </c>
@@ -1624,7 +1639,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="19" t="s">
         <v>19</v>
@@ -1648,7 +1663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>22</v>
       </c>
@@ -1662,7 +1677,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="19" t="s">
         <v>23</v>
@@ -1684,7 +1699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="19" t="s">
         <v>25</v>
@@ -1706,7 +1721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="19" t="s">
         <v>26</v>
@@ -1728,7 +1743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="19" t="s">
         <v>27</v>
@@ -1750,7 +1765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="19" t="s">
         <v>28</v>
@@ -1772,7 +1787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>29</v>
       </c>
@@ -1786,7 +1801,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="19" t="s">
         <v>30</v>
@@ -1808,7 +1823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="19" t="s">
         <v>31</v>
@@ -1830,7 +1845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="19" t="s">
         <v>32</v>
@@ -1852,7 +1867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="19" t="s">
         <v>33</v>
@@ -1874,7 +1889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="19" t="s">
         <v>34</v>
@@ -1896,7 +1911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="19" t="s">
         <v>35</v>
@@ -1918,7 +1933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="19" t="s">
         <v>36</v>
@@ -1940,7 +1955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="19" t="s">
         <v>37</v>
@@ -1962,7 +1977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="19" t="s">
         <v>38</v>
@@ -1984,7 +1999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="19" t="s">
         <v>39</v>
@@ -2006,7 +2021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>40</v>
       </c>
@@ -2020,7 +2035,7 @@
       <c r="I28" s="10"/>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>41</v>
       </c>
@@ -2034,7 +2049,7 @@
       <c r="I29" s="10"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="19" t="s">
         <v>42</v>
@@ -2062,7 +2077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="19" t="s">
         <v>46</v>
@@ -2088,32 +2103,32 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="19" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="18"/>
-    </row>
-    <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G32" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>43</v>
@@ -2122,37 +2137,33 @@
         <v>20</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F33" s="14"/>
-      <c r="G33" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="17"/>
-      <c r="J33" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14" t="s">
-        <v>115</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="14"/>
       <c r="G34" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H34" s="16" t="s">
         <v>13</v>
@@ -2162,10 +2173,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>54</v>
@@ -2178,7 +2189,7 @@
         <v>115</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H35" s="16" t="s">
         <v>13</v>
@@ -2188,50 +2199,50 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="35" t="s">
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="11"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="17"/>
-      <c r="J37" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="21"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>54</v>
@@ -2244,7 +2255,7 @@
         <v>115</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>13</v>
@@ -2254,21 +2265,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="F39" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="G39" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H39" s="16" t="s">
         <v>13</v>
@@ -2278,10 +2291,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>54</v>
@@ -2292,7 +2305,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
       <c r="G40" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H40" s="16" t="s">
         <v>13</v>
@@ -2302,10 +2315,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>54</v>
@@ -2316,7 +2329,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H41" s="16" t="s">
         <v>13</v>
@@ -2326,10 +2339,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>54</v>
@@ -2340,7 +2353,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="G42" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H42" s="16" t="s">
         <v>13</v>
@@ -2350,51 +2363,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="35" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="11"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="17"/>
-      <c r="J44" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B44" s="21"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>15</v>
@@ -2402,7 +2415,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>13</v>
@@ -2412,10 +2425,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>54</v>
@@ -2426,7 +2439,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="G46" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>13</v>
@@ -2436,10 +2449,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>54</v>
@@ -2450,78 +2463,74 @@
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
       <c r="G47" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="17"/>
+      <c r="J47" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="16"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="18"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="35" t="s">
+      <c r="H48" s="16"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="18"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="11"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="13"/>
-      <c r="B49" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H49" s="16"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="18"/>
-    </row>
-    <row r="50" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B49" s="21"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>84</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="H50" s="16"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="18"/>
+    </row>
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="19" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>43</v>
@@ -2530,11 +2539,11 @@
         <v>20</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H51" s="16" t="s">
         <v>13</v>
@@ -2546,23 +2555,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14" t="s">
-        <v>115</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" s="14"/>
       <c r="G52" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H52" s="16" t="s">
         <v>13</v>
@@ -2574,10 +2583,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>54</v>
@@ -2586,9 +2595,11 @@
         <v>55</v>
       </c>
       <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+      <c r="F53" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="G53" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H53" s="16" t="s">
         <v>13</v>
@@ -2600,21 +2611,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
       <c r="G54" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>13</v>
@@ -2626,49 +2637,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E55" s="14"/>
-      <c r="F55" s="14" t="s">
-        <v>115</v>
-      </c>
+      <c r="F55" s="14"/>
       <c r="G55" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="J55" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="19" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
+      <c r="F56" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="G56" s="15" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="H56" s="16" t="s">
         <v>13</v>
@@ -2680,47 +2691,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
+      <c r="F57" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="G57" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I57" s="17" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="J57" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
       <c r="G58" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H58" s="16" t="s">
         <v>13</v>
@@ -2732,37 +2745,47 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="11"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="E60" s="14"/>
-      <c r="F60" s="14" t="s">
-        <v>115</v>
-      </c>
+      <c r="F60" s="14"/>
       <c r="G60" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H60" s="16" t="s">
         <v>13</v>
@@ -2774,27 +2797,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="34"/>
-    </row>
-    <row r="62" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="21"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="19" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>55</v>
@@ -2804,94 +2827,100 @@
         <v>115</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="H62" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I62" s="17"/>
+      <c r="I62" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="J62" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
-      <c r="B63" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" s="17" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="29"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="34"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="H63" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="17"/>
-      <c r="J63" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="11"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D64" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="17"/>
+      <c r="J64" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="14"/>
+        <v>120</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="F65" s="14"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="G65" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H65" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="17"/>
       <c r="J65" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="13"/>
-      <c r="B66" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J66" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="21"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="11"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="17"/>
@@ -2906,10 +2935,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="19" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="17"/>
@@ -2924,13 +2953,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
+        <v>111</v>
+      </c>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
       <c r="G69" s="15"/>
@@ -2942,19 +2971,55 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="23"/>
-      <c r="B70" s="24" t="s">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J71" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="23"/>
+      <c r="B72" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="23"/>
-      <c r="I70" s="27"/>
-      <c r="J70" s="28"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>